<commit_message>
added additional puzzles - 7 total to include the test puzzle (2x2)
</commit_message>
<xml_diff>
--- a/Puzzle Solutions/Puzzle Template.xlsx
+++ b/Puzzle Solutions/Puzzle Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csuser\Desktop\pc\Puzzle Solutions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csuser\Desktop\PC\Puzzle Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7A35B18-F5BD-41FD-9A9F-07986D51A409}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F81AFC-5FF7-44EC-9504-82C41A2B1545}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625" xr2:uid="{3A8D592D-A54F-4664-B72A-B5048B2C78F4}"/>
   </bookViews>
@@ -25,9 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Puzzle 1</t>
+    <t>Puzzle A</t>
   </si>
 </sst>
 </file>
@@ -43,12 +43,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -78,9 +84,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,105 +441,233 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="C3" s="2">
+        <v>57</v>
+      </c>
+      <c r="D3" s="1">
+        <v>58</v>
+      </c>
+      <c r="E3" s="1">
+        <v>59</v>
+      </c>
+      <c r="F3" s="1">
+        <v>60</v>
+      </c>
+      <c r="G3" s="1">
+        <v>61</v>
+      </c>
+      <c r="H3" s="2">
+        <v>62</v>
+      </c>
+      <c r="I3" s="1">
+        <v>63</v>
+      </c>
+      <c r="J3" s="2">
+        <v>64</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="C4" s="1">
+        <v>56</v>
+      </c>
+      <c r="D4" s="1">
+        <v>33</v>
+      </c>
+      <c r="E4" s="2">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1">
+        <v>31</v>
+      </c>
+      <c r="G4" s="1">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1">
+        <v>29</v>
+      </c>
+      <c r="I4" s="1">
+        <v>28</v>
+      </c>
+      <c r="J4" s="1">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="C5" s="1">
+        <v>55</v>
+      </c>
+      <c r="D5" s="1">
+        <v>34</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>21</v>
+      </c>
+      <c r="H5" s="2">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1">
+        <v>23</v>
+      </c>
+      <c r="J5" s="1">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="C6" s="1">
+        <v>54</v>
+      </c>
+      <c r="D6" s="2">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1">
+        <v>19</v>
+      </c>
+      <c r="I6" s="1">
+        <v>24</v>
+      </c>
+      <c r="J6" s="1">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="C7" s="2">
+        <v>53</v>
+      </c>
+      <c r="D7" s="1">
+        <v>52</v>
+      </c>
+      <c r="E7" s="1">
+        <v>37</v>
+      </c>
+      <c r="F7" s="2">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1">
+        <v>18</v>
+      </c>
+      <c r="I7" s="1">
+        <v>17</v>
+      </c>
+      <c r="J7" s="2">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="C8" s="1">
+        <v>50</v>
+      </c>
+      <c r="D8" s="1">
+        <v>51</v>
+      </c>
+      <c r="E8" s="1">
+        <v>38</v>
+      </c>
+      <c r="F8" s="1">
+        <v>39</v>
+      </c>
+      <c r="G8" s="1">
+        <v>6</v>
+      </c>
+      <c r="H8" s="1">
+        <v>7</v>
+      </c>
+      <c r="I8" s="1">
+        <v>14</v>
+      </c>
+      <c r="J8" s="1">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="C9" s="1">
+        <v>49</v>
+      </c>
+      <c r="D9" s="1">
+        <v>46</v>
+      </c>
+      <c r="E9" s="1">
+        <v>45</v>
+      </c>
+      <c r="F9" s="1">
+        <v>40</v>
+      </c>
+      <c r="G9" s="1">
+        <v>41</v>
+      </c>
+      <c r="H9" s="2">
+        <v>8</v>
+      </c>
+      <c r="I9" s="1">
+        <v>13</v>
+      </c>
+      <c r="J9" s="1">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="C10" s="2">
+        <v>48</v>
+      </c>
+      <c r="D10" s="1">
+        <v>47</v>
+      </c>
+      <c r="E10" s="2">
+        <v>44</v>
+      </c>
+      <c r="F10" s="1">
+        <v>43</v>
+      </c>
+      <c r="G10" s="1">
+        <v>42</v>
+      </c>
+      <c r="H10" s="1">
+        <v>9</v>
+      </c>
+      <c r="I10" s="1">
+        <v>10</v>
+      </c>
+      <c r="J10" s="2">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>